<commit_message>
Added demo data T30177TT
</commit_message>
<xml_diff>
--- a/demo data/HDX-MS raw data/CF-HDX time points.xlsx
+++ b/demo data/HDX-MS raw data/CF-HDX time points.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubordeauxfr-my.sharepoint.com/personal/eric_largy_u-bordeaux_fr/Documents/Git/OligoR_reboot/demo data/HDX-MS processed data/PhenDC3 cplx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubordeauxfr-my.sharepoint.com/personal/eric_largy_u-bordeaux_fr/Documents/Git/OligoR_reboot/demo data/HDX-MS raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D6D88CC-D9B7-4F42-9D70-CB1EC2C950A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{1D6D88CC-D9B7-4F42-9D70-CB1EC2C950A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1091420-5ED5-4E24-B750-CD55AD61A961}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{B62CD297-82F9-417D-AA6F-874AE1DC3828}"/>
   </bookViews>
@@ -33,12 +33,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>file number</t>
   </si>
   <si>
     <t>exchange time (s)</t>
+  </si>
+  <si>
+    <t>23TAG</t>
+  </si>
+  <si>
+    <t>T30177-TT</t>
   </si>
 </sst>
 </file>
@@ -74,8 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,187 +400,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243A7411-54FB-420E-AC90-D40A4F4001D3}">
-  <dimension ref="F6:G26"/>
+  <dimension ref="F5:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2">
+        <v>3.3079570258276223</v>
+      </c>
+    </row>
+    <row r="8" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F8">
         <v>2</v>
       </c>
       <c r="G8">
         <v>3.72</v>
       </c>
-    </row>
-    <row r="9" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="2">
+        <v>4.1349462822845275</v>
+      </c>
+    </row>
+    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9">
         <v>4.6500000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="2">
+        <v>4.7256528940394604</v>
+      </c>
+    </row>
+    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>4</v>
       </c>
       <c r="G10">
         <v>5.31</v>
       </c>
-    </row>
-    <row r="11" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="2">
+        <v>5.5132617097127037</v>
+      </c>
+    </row>
+    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>5</v>
       </c>
       <c r="G11">
         <v>9.82</v>
       </c>
-    </row>
-    <row r="12" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="2">
+        <v>11.073968936476858</v>
+      </c>
+    </row>
+    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>6</v>
       </c>
       <c r="G12">
         <v>12.27</v>
       </c>
-    </row>
-    <row r="13" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="2">
+        <v>12.655964498830695</v>
+      </c>
+    </row>
+    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>7</v>
       </c>
       <c r="G13">
         <v>14.02</v>
       </c>
-    </row>
-    <row r="14" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="2">
+        <v>14.765291915302477</v>
+      </c>
+    </row>
+    <row r="14" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F14">
         <v>8</v>
       </c>
       <c r="G14">
         <v>16.36</v>
       </c>
-    </row>
-    <row r="15" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="2">
+        <v>25.718112194695514</v>
+      </c>
+    </row>
+    <row r="15" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>9</v>
       </c>
       <c r="G15">
         <v>19.63</v>
       </c>
-    </row>
-    <row r="16" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2">
+        <v>29.392128222509157</v>
+      </c>
+    </row>
+    <row r="16" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>10</v>
       </c>
       <c r="G16">
         <v>30.74</v>
       </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2">
+        <v>34.290816259594017</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>11</v>
       </c>
       <c r="G17">
         <v>38.43</v>
       </c>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2">
+        <v>53.821039482092587</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>12</v>
       </c>
       <c r="G18">
         <v>43.92</v>
       </c>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="2">
+        <v>61.509759408105815</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>13</v>
       </c>
       <c r="G19">
         <v>51.24</v>
       </c>
-    </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="2">
+        <v>71.761385976123449</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>14</v>
       </c>
       <c r="G20">
         <v>61.48</v>
       </c>
-    </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="2">
+        <v>80.315545955149929</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>15</v>
       </c>
       <c r="G21">
         <v>55.95</v>
       </c>
-    </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="2">
+        <v>91.789195377314215</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>16</v>
       </c>
       <c r="G22">
         <v>69.930000000000007</v>
       </c>
-    </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="2">
+        <v>107.08739460686658</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>17</v>
       </c>
       <c r="G23">
         <v>79.92</v>
       </c>
-    </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2">
+        <v>136.13097058327409</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F24">
         <v>18</v>
       </c>
       <c r="G24">
         <v>93.24</v>
       </c>
-    </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2">
+        <v>163.35716469992892</v>
+      </c>
+    </row>
+    <row r="25" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F25">
         <v>19</v>
       </c>
       <c r="G25">
         <v>111.89</v>
       </c>
-    </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="2">
+        <v>201.49860328019528</v>
+      </c>
+    </row>
+    <row r="26" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F26">
         <v>20</v>
       </c>
       <c r="G26">
         <v>139.87</v>
       </c>
+      <c r="H26" s="2">
+        <v>235.08170382689448</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G5:H5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>